<commit_message>
Add Elite Team strategy and fix API key exposure
Security:
- Remove plist files containing API key from git tracking
- Add backend/automation/*.plist to .gitignore

Features:
- Add Elite Team strategy (top 25% by win% in good recent form)
- New /api/elite-teams endpoint in predictions API
- New EliteTeamsScreen in frontend app
- Add network strength and spread coverage analysis notebooks

Data:
- Update season results with latest games
- Add network ratings CSV files

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/backend/data/results/nba_season_results.xlsx
+++ b/backend/data/results/nba_season_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G504"/>
+  <dimension ref="A1:G538"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14055,6 +14055,924 @@
         <v>3.5</v>
       </c>
     </row>
+    <row r="505">
+      <c r="A505" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Washington Wizards</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>Brooklyn Nets</t>
+        </is>
+      </c>
+      <c r="D505" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="E505" t="n">
+        <v>119</v>
+      </c>
+      <c r="F505" t="n">
+        <v>99</v>
+      </c>
+      <c r="G505" t="n">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="D506" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E506" t="n">
+        <v>113</v>
+      </c>
+      <c r="F506" t="n">
+        <v>123</v>
+      </c>
+      <c r="G506" t="n">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="D507" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="E507" t="n">
+        <v>99</v>
+      </c>
+      <c r="F507" t="n">
+        <v>111</v>
+      </c>
+      <c r="G507" t="n">
+        <v>-16.5</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="D508" t="n">
+        <v>-13.5</v>
+      </c>
+      <c r="E508" t="n">
+        <v>113</v>
+      </c>
+      <c r="F508" t="n">
+        <v>108</v>
+      </c>
+      <c r="G508" t="n">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="D509" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E509" t="n">
+        <v>121</v>
+      </c>
+      <c r="F509" t="n">
+        <v>114</v>
+      </c>
+      <c r="G509" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="D510" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E510" t="n">
+        <v>122</v>
+      </c>
+      <c r="F510" t="n">
+        <v>121</v>
+      </c>
+      <c r="G510" t="n">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>New Orleans Pelicans</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="D511" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E511" t="n">
+        <v>109</v>
+      </c>
+      <c r="F511" t="n">
+        <v>122</v>
+      </c>
+      <c r="G511" t="n">
+        <v>-9.5</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="D512" t="n">
+        <v>-13.5</v>
+      </c>
+      <c r="E512" t="n">
+        <v>129</v>
+      </c>
+      <c r="F512" t="n">
+        <v>102</v>
+      </c>
+      <c r="G512" t="n">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Golden State Warriors</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>Oklahoma City Thunder</t>
+        </is>
+      </c>
+      <c r="D513" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="E513" t="n">
+        <v>94</v>
+      </c>
+      <c r="F513" t="n">
+        <v>131</v>
+      </c>
+      <c r="G513" t="n">
+        <v>-23.5</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="D514" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E514" t="n">
+        <v>128</v>
+      </c>
+      <c r="F514" t="n">
+        <v>121</v>
+      </c>
+      <c r="G514" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>Minnesota Timberwolves</t>
+        </is>
+      </c>
+      <c r="D515" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E515" t="n">
+        <v>115</v>
+      </c>
+      <c r="F515" t="n">
+        <v>125</v>
+      </c>
+      <c r="G515" t="n">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>Philadelphia 76ers</t>
+        </is>
+      </c>
+      <c r="D516" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="E516" t="n">
+        <v>119</v>
+      </c>
+      <c r="F516" t="n">
+        <v>130</v>
+      </c>
+      <c r="G516" t="n">
+        <v>-14.5</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Toronto Raptors</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="D517" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E517" t="n">
+        <v>134</v>
+      </c>
+      <c r="F517" t="n">
+        <v>117</v>
+      </c>
+      <c r="G517" t="n">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="D518" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="E518" t="n">
+        <v>99</v>
+      </c>
+      <c r="F518" t="n">
+        <v>112</v>
+      </c>
+      <c r="G518" t="n">
+        <v>-15.5</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="D519" t="n">
+        <v>-8.5</v>
+      </c>
+      <c r="E519" t="n">
+        <v>110</v>
+      </c>
+      <c r="F519" t="n">
+        <v>115</v>
+      </c>
+      <c r="G519" t="n">
+        <v>-13.5</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Dallas Mavericks</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>Houston Rockets</t>
+        </is>
+      </c>
+      <c r="D520" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E520" t="n">
+        <v>110</v>
+      </c>
+      <c r="F520" t="n">
+        <v>104</v>
+      </c>
+      <c r="G520" t="n">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Golden State Warriors</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D521" t="n">
+        <v>-12.5</v>
+      </c>
+      <c r="E521" t="n">
+        <v>123</v>
+      </c>
+      <c r="F521" t="n">
+        <v>114</v>
+      </c>
+      <c r="G521" t="n">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="2" t="n">
+        <v>46025</v>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="D522" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="E522" t="n">
+        <v>115</v>
+      </c>
+      <c r="F522" t="n">
+        <v>146</v>
+      </c>
+      <c r="G522" t="n">
+        <v>-32.5</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>Detroit Pistons</t>
+        </is>
+      </c>
+      <c r="D523" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="E523" t="n">
+        <v>110</v>
+      </c>
+      <c r="F523" t="n">
+        <v>114</v>
+      </c>
+      <c r="G523" t="n">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="D524" t="n">
+        <v>-6.5</v>
+      </c>
+      <c r="E524" t="n">
+        <v>135</v>
+      </c>
+      <c r="F524" t="n">
+        <v>127</v>
+      </c>
+      <c r="G524" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Brooklyn Nets</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="D525" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E525" t="n">
+        <v>127</v>
+      </c>
+      <c r="F525" t="n">
+        <v>115</v>
+      </c>
+      <c r="G525" t="n">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Washington Wizards</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>Minnesota Timberwolves</t>
+        </is>
+      </c>
+      <c r="D526" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E526" t="n">
+        <v>115</v>
+      </c>
+      <c r="F526" t="n">
+        <v>141</v>
+      </c>
+      <c r="G526" t="n">
+        <v>-15.5</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>New Orleans Pelicans</t>
+        </is>
+      </c>
+      <c r="D527" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="E527" t="n">
+        <v>125</v>
+      </c>
+      <c r="F527" t="n">
+        <v>106</v>
+      </c>
+      <c r="G527" t="n">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>Oklahoma City Thunder</t>
+        </is>
+      </c>
+      <c r="D528" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E528" t="n">
+        <v>108</v>
+      </c>
+      <c r="F528" t="n">
+        <v>105</v>
+      </c>
+      <c r="G528" t="n">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="D529" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E529" t="n">
+        <v>98</v>
+      </c>
+      <c r="F529" t="n">
+        <v>115</v>
+      </c>
+      <c r="G529" t="n">
+        <v>-10.5</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="2" t="n">
+        <v>46026</v>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="D530" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E530" t="n">
+        <v>120</v>
+      </c>
+      <c r="F530" t="n">
+        <v>114</v>
+      </c>
+      <c r="G530" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Detroit Pistons</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="D531" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E531" t="n">
+        <v>121</v>
+      </c>
+      <c r="F531" t="n">
+        <v>90</v>
+      </c>
+      <c r="G531" t="n">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Toronto Raptors</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="D532" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="E532" t="n">
+        <v>118</v>
+      </c>
+      <c r="F532" t="n">
+        <v>100</v>
+      </c>
+      <c r="G532" t="n">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="D533" t="n">
+        <v>-10.5</v>
+      </c>
+      <c r="E533" t="n">
+        <v>115</v>
+      </c>
+      <c r="F533" t="n">
+        <v>101</v>
+      </c>
+      <c r="G533" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Oklahoma City Thunder</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="D534" t="n">
+        <v>-15.5</v>
+      </c>
+      <c r="E534" t="n">
+        <v>97</v>
+      </c>
+      <c r="F534" t="n">
+        <v>124</v>
+      </c>
+      <c r="G534" t="n">
+        <v>-42.5</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Houston Rockets</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="D535" t="n">
+        <v>-8.5</v>
+      </c>
+      <c r="E535" t="n">
+        <v>100</v>
+      </c>
+      <c r="F535" t="n">
+        <v>97</v>
+      </c>
+      <c r="G535" t="n">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Philadelphia 76ers</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="D536" t="n">
+        <v>-14.5</v>
+      </c>
+      <c r="E536" t="n">
+        <v>124</v>
+      </c>
+      <c r="F536" t="n">
+        <v>125</v>
+      </c>
+      <c r="G536" t="n">
+        <v>-15.5</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>Golden State Warriors</t>
+        </is>
+      </c>
+      <c r="D537" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E537" t="n">
+        <v>103</v>
+      </c>
+      <c r="F537" t="n">
+        <v>102</v>
+      </c>
+      <c r="G537" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D538" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E538" t="n">
+        <v>137</v>
+      </c>
+      <c r="F538" t="n">
+        <v>117</v>
+      </c>
+      <c r="G538" t="n">
+        <v>14.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add sample size guardrails to insight engine
- Lower slider minimum to 5 (user's minimum acceptable sample)
- Add caution note for patterns with <30 samples
- Update confidence calculation to require both sample size AND edge thresholds
- High: 50+ samples AND 8%+ edge
- Medium: 30+ samples AND 5%+ edge
- Low: everything else (use with caution)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/backend/data/results/nba_season_results.xlsx
+++ b/backend/data/results/nba_season_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G538"/>
+  <dimension ref="A1:G556"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14973,6 +14973,492 @@
         <v>14.5</v>
       </c>
     </row>
+    <row r="539">
+      <c r="A539" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="D539" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E539" t="n">
+        <v>116</v>
+      </c>
+      <c r="F539" t="n">
+        <v>120</v>
+      </c>
+      <c r="G539" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Washington Wizards</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="D540" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E540" t="n">
+        <v>120</v>
+      </c>
+      <c r="F540" t="n">
+        <v>112</v>
+      </c>
+      <c r="G540" t="n">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>New Orleans Pelicans</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="D541" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E541" t="n">
+        <v>103</v>
+      </c>
+      <c r="F541" t="n">
+        <v>111</v>
+      </c>
+      <c r="G541" t="n">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="D542" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E542" t="n">
+        <v>106</v>
+      </c>
+      <c r="F542" t="n">
+        <v>105</v>
+      </c>
+      <c r="G542" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Minnesota Timberwolves</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+      <c r="D543" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E543" t="n">
+        <v>122</v>
+      </c>
+      <c r="F543" t="n">
+        <v>94</v>
+      </c>
+      <c r="G543" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>Dallas Mavericks</t>
+        </is>
+      </c>
+      <c r="D544" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E544" t="n">
+        <v>98</v>
+      </c>
+      <c r="F544" t="n">
+        <v>100</v>
+      </c>
+      <c r="G544" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Detroit Pistons</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="D545" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="E545" t="n">
+        <v>108</v>
+      </c>
+      <c r="F545" t="n">
+        <v>93</v>
+      </c>
+      <c r="G545" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Philadelphia 76ers</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>Washington Wizards</t>
+        </is>
+      </c>
+      <c r="D546" t="n">
+        <v>-16.5</v>
+      </c>
+      <c r="E546" t="n">
+        <v>131</v>
+      </c>
+      <c r="F546" t="n">
+        <v>110</v>
+      </c>
+      <c r="G546" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>Toronto Raptors</t>
+        </is>
+      </c>
+      <c r="D547" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E547" t="n">
+        <v>96</v>
+      </c>
+      <c r="F547" t="n">
+        <v>97</v>
+      </c>
+      <c r="G547" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="D548" t="n">
+        <v>-10.5</v>
+      </c>
+      <c r="E548" t="n">
+        <v>110</v>
+      </c>
+      <c r="F548" t="n">
+        <v>114</v>
+      </c>
+      <c r="G548" t="n">
+        <v>-14.5</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>New Orleans Pelicans</t>
+        </is>
+      </c>
+      <c r="D549" t="n">
+        <v>-11.5</v>
+      </c>
+      <c r="E549" t="n">
+        <v>117</v>
+      </c>
+      <c r="F549" t="n">
+        <v>100</v>
+      </c>
+      <c r="G549" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Brooklyn Nets</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="D550" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E550" t="n">
+        <v>103</v>
+      </c>
+      <c r="F550" t="n">
+        <v>104</v>
+      </c>
+      <c r="G550" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="D551" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="E551" t="n">
+        <v>123</v>
+      </c>
+      <c r="F551" t="n">
+        <v>111</v>
+      </c>
+      <c r="G551" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="D552" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E552" t="n">
+        <v>98</v>
+      </c>
+      <c r="F552" t="n">
+        <v>117</v>
+      </c>
+      <c r="G552" t="n">
+        <v>-13.5</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Oklahoma City Thunder</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D553" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="E553" t="n">
+        <v>129</v>
+      </c>
+      <c r="F553" t="n">
+        <v>125</v>
+      </c>
+      <c r="G553" t="n">
+        <v>-15.5</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="D554" t="n">
+        <v>-8.5</v>
+      </c>
+      <c r="E554" t="n">
+        <v>107</v>
+      </c>
+      <c r="F554" t="n">
+        <v>91</v>
+      </c>
+      <c r="G554" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Golden State Warriors</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="D555" t="n">
+        <v>-6.5</v>
+      </c>
+      <c r="E555" t="n">
+        <v>120</v>
+      </c>
+      <c r="F555" t="n">
+        <v>113</v>
+      </c>
+      <c r="G555" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>Houston Rockets</t>
+        </is>
+      </c>
+      <c r="D556" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E556" t="n">
+        <v>103</v>
+      </c>
+      <c r="F556" t="n">
+        <v>102</v>
+      </c>
+      <c r="G556" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add over/under (totals) support to games database
- Add closing_total and total_result columns to games table
- Add total and total_source columns to todays_games table
- Update Lambda functions to collect totals from Odds API
- Add migration script for totals columns
- Add backfill script for historical totals data
- Add generate_historical_ratings Lambda function
- Update notebooks with latest analysis
- Fix SQLite connection pooling for mixed API usage

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/backend/data/results/nba_season_results.xlsx
+++ b/backend/data/results/nba_season_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G556"/>
+  <dimension ref="A1:G591"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15459,6 +15459,951 @@
         <v>8.5</v>
       </c>
     </row>
+    <row r="557">
+      <c r="A557" s="2" t="n">
+        <v>46030</v>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="D557" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="E557" t="n">
+        <v>112</v>
+      </c>
+      <c r="F557" t="n">
+        <v>114</v>
+      </c>
+      <c r="G557" t="n">
+        <v>-6.5</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="2" t="n">
+        <v>46030</v>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Minnesota Timberwolves</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="D558" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="E558" t="n">
+        <v>131</v>
+      </c>
+      <c r="F558" t="n">
+        <v>122</v>
+      </c>
+      <c r="G558" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="2" t="n">
+        <v>46030</v>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>Dallas Mavericks</t>
+        </is>
+      </c>
+      <c r="D559" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E559" t="n">
+        <v>116</v>
+      </c>
+      <c r="F559" t="n">
+        <v>114</v>
+      </c>
+      <c r="G559" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>Toronto Raptors</t>
+        </is>
+      </c>
+      <c r="D560" t="n">
+        <v>-9.5</v>
+      </c>
+      <c r="E560" t="n">
+        <v>125</v>
+      </c>
+      <c r="F560" t="n">
+        <v>117</v>
+      </c>
+      <c r="G560" t="n">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>Philadelphia 76ers</t>
+        </is>
+      </c>
+      <c r="D561" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E561" t="n">
+        <v>91</v>
+      </c>
+      <c r="F561" t="n">
+        <v>103</v>
+      </c>
+      <c r="G561" t="n">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Washington Wizards</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>New Orleans Pelicans</t>
+        </is>
+      </c>
+      <c r="D562" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E562" t="n">
+        <v>107</v>
+      </c>
+      <c r="F562" t="n">
+        <v>128</v>
+      </c>
+      <c r="G562" t="n">
+        <v>-17.5</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Brooklyn Nets</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="D563" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E563" t="n">
+        <v>105</v>
+      </c>
+      <c r="F563" t="n">
+        <v>121</v>
+      </c>
+      <c r="G563" t="n">
+        <v>-10.5</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>Oklahoma City Thunder</t>
+        </is>
+      </c>
+      <c r="D564" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E564" t="n">
+        <v>116</v>
+      </c>
+      <c r="F564" t="n">
+        <v>117</v>
+      </c>
+      <c r="G564" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="D565" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E565" t="n">
+        <v>112</v>
+      </c>
+      <c r="F565" t="n">
+        <v>107</v>
+      </c>
+      <c r="G565" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="D566" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E566" t="n">
+        <v>87</v>
+      </c>
+      <c r="F566" t="n">
+        <v>110</v>
+      </c>
+      <c r="G566" t="n">
+        <v>-19.5</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Golden State Warriors</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="D567" t="n">
+        <v>-15.5</v>
+      </c>
+      <c r="E567" t="n">
+        <v>137</v>
+      </c>
+      <c r="F567" t="n">
+        <v>103</v>
+      </c>
+      <c r="G567" t="n">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>Houston Rockets</t>
+        </is>
+      </c>
+      <c r="D568" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E568" t="n">
+        <v>111</v>
+      </c>
+      <c r="F568" t="n">
+        <v>105</v>
+      </c>
+      <c r="G568" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="2" t="n">
+        <v>46031</v>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="D569" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="E569" t="n">
+        <v>101</v>
+      </c>
+      <c r="F569" t="n">
+        <v>105</v>
+      </c>
+      <c r="G569" t="n">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="2" t="n">
+        <v>46032</v>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>Minnesota Timberwolves</t>
+        </is>
+      </c>
+      <c r="D570" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="E570" t="n">
+        <v>146</v>
+      </c>
+      <c r="F570" t="n">
+        <v>134</v>
+      </c>
+      <c r="G570" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="2" t="n">
+        <v>46032</v>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+      <c r="D571" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E571" t="n">
+        <v>123</v>
+      </c>
+      <c r="F571" t="n">
+        <v>99</v>
+      </c>
+      <c r="G571" t="n">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="2" t="n">
+        <v>46032</v>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Detroit Pistons</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="D572" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="E572" t="n">
+        <v>92</v>
+      </c>
+      <c r="F572" t="n">
+        <v>98</v>
+      </c>
+      <c r="G572" t="n">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="2" t="n">
+        <v>46032</v>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="D573" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E573" t="n">
+        <v>95</v>
+      </c>
+      <c r="F573" t="n">
+        <v>100</v>
+      </c>
+      <c r="G573" t="n">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="2" t="n">
+        <v>46032</v>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>Dallas Mavericks</t>
+        </is>
+      </c>
+      <c r="D574" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="E574" t="n">
+        <v>125</v>
+      </c>
+      <c r="F574" t="n">
+        <v>107</v>
+      </c>
+      <c r="G574" t="n">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="2" t="n">
+        <v>46032</v>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="D575" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E575" t="n">
+        <v>95</v>
+      </c>
+      <c r="F575" t="n">
+        <v>150</v>
+      </c>
+      <c r="G575" t="n">
+        <v>-48.5</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Orlando Magic</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>New Orleans Pelicans</t>
+        </is>
+      </c>
+      <c r="D576" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="E576" t="n">
+        <v>128</v>
+      </c>
+      <c r="F576" t="n">
+        <v>118</v>
+      </c>
+      <c r="G576" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Memphis Grizzlies</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>Brooklyn Nets</t>
+        </is>
+      </c>
+      <c r="D577" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="E577" t="n">
+        <v>103</v>
+      </c>
+      <c r="F577" t="n">
+        <v>98</v>
+      </c>
+      <c r="G577" t="n">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Toronto Raptors</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>Philadelphia 76ers</t>
+        </is>
+      </c>
+      <c r="D578" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E578" t="n">
+        <v>116</v>
+      </c>
+      <c r="F578" t="n">
+        <v>115</v>
+      </c>
+      <c r="G578" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>New York Knicks</t>
+        </is>
+      </c>
+      <c r="D579" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E579" t="n">
+        <v>114</v>
+      </c>
+      <c r="F579" t="n">
+        <v>123</v>
+      </c>
+      <c r="G579" t="n">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Oklahoma City Thunder</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>Miami Heat</t>
+        </is>
+      </c>
+      <c r="D580" t="n">
+        <v>-14.5</v>
+      </c>
+      <c r="E580" t="n">
+        <v>124</v>
+      </c>
+      <c r="F580" t="n">
+        <v>112</v>
+      </c>
+      <c r="G580" t="n">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Minnesota Timberwolves</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>San Antonio Spurs</t>
+        </is>
+      </c>
+      <c r="D581" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="E581" t="n">
+        <v>104</v>
+      </c>
+      <c r="F581" t="n">
+        <v>103</v>
+      </c>
+      <c r="G581" t="n">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Denver Nuggets</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="D582" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E582" t="n">
+        <v>108</v>
+      </c>
+      <c r="F582" t="n">
+        <v>104</v>
+      </c>
+      <c r="G582" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Phoenix Suns</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>Washington Wizards</t>
+        </is>
+      </c>
+      <c r="D583" t="n">
+        <v>-15.5</v>
+      </c>
+      <c r="E583" t="n">
+        <v>112</v>
+      </c>
+      <c r="F583" t="n">
+        <v>93</v>
+      </c>
+      <c r="G583" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Golden State Warriors</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>Atlanta Hawks</t>
+        </is>
+      </c>
+      <c r="D584" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="E584" t="n">
+        <v>111</v>
+      </c>
+      <c r="F584" t="n">
+        <v>124</v>
+      </c>
+      <c r="G584" t="n">
+        <v>-20.5</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>Houston Rockets</t>
+        </is>
+      </c>
+      <c r="D585" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="E585" t="n">
+        <v>111</v>
+      </c>
+      <c r="F585" t="n">
+        <v>98</v>
+      </c>
+      <c r="G585" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>Utah Jazz</t>
+        </is>
+      </c>
+      <c r="D586" t="n">
+        <v>-13.5</v>
+      </c>
+      <c r="E586" t="n">
+        <v>112</v>
+      </c>
+      <c r="F586" t="n">
+        <v>123</v>
+      </c>
+      <c r="G586" t="n">
+        <v>-24.5</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Indiana Pacers</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="D587" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E587" t="n">
+        <v>98</v>
+      </c>
+      <c r="F587" t="n">
+        <v>96</v>
+      </c>
+      <c r="G587" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Toronto Raptors</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>Philadelphia 76ers</t>
+        </is>
+      </c>
+      <c r="D588" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E588" t="n">
+        <v>102</v>
+      </c>
+      <c r="F588" t="n">
+        <v>115</v>
+      </c>
+      <c r="G588" t="n">
+        <v>-9.5</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Dallas Mavericks</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>Brooklyn Nets</t>
+        </is>
+      </c>
+      <c r="D589" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="E589" t="n">
+        <v>113</v>
+      </c>
+      <c r="F589" t="n">
+        <v>105</v>
+      </c>
+      <c r="G589" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Sacramento Kings</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="D590" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E590" t="n">
+        <v>124</v>
+      </c>
+      <c r="F590" t="n">
+        <v>112</v>
+      </c>
+      <c r="G590" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Los Angeles Clippers</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>Charlotte Hornets</t>
+        </is>
+      </c>
+      <c r="D591" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="E591" t="n">
+        <v>117</v>
+      </c>
+      <c r="F591" t="n">
+        <v>109</v>
+      </c>
+      <c r="G591" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>